<commit_message>
Add X-15 max Q
</commit_message>
<xml_diff>
--- a/SpaceX - JCSAT14 Launch.xlsx
+++ b/SpaceX - JCSAT14 Launch.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\SpaceX-JCSAT14-Launch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\MaxQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13035" xr2:uid="{D5B2B441-1BD3-4769-9F13-9212EC359BD6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13035" activeTab="1" xr2:uid="{D5B2B441-1BD3-4769-9F13-9212EC359BD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Time</t>
   </si>
@@ -448,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AD44BD-DC53-4AB9-91BC-FB75E6A0B3E5}">
   <dimension ref="A1:S163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="J83" sqref="J83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4056,6 +4056,9 @@
         <f t="shared" si="13"/>
         <v>14521.666666666664</v>
       </c>
+      <c r="J82" t="s">
+        <v>6</v>
+      </c>
       <c r="K82">
         <f t="shared" si="14"/>
         <v>31.69985844186002</v>
@@ -7663,8 +7666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11BF133B-594B-48C5-AE55-9FDEC5E2D735}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8011,6 +8014,9 @@
         <f t="shared" si="1"/>
         <v>33313.276857283949</v>
       </c>
+      <c r="K12" t="s">
+        <v>6</v>
+      </c>
       <c r="L12">
         <f t="shared" si="2"/>
         <v>39</v>

</xml_diff>